<commit_message>
excel file change with 2 more questions & uppsats added abstract, new result in interview
</commit_message>
<xml_diff>
--- a/interview/interviewScores.xlsx
+++ b/interview/interviewScores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14680" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
   <si>
     <t>Frågor</t>
   </si>
@@ -122,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -164,6 +164,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -182,7 +195,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -190,8 +203,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -205,14 +224,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+  <cellStyles count="13">
+    <cellStyle name="Följd hyperlänk" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Följd hyperlänk" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlänk" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -542,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -608,7 +637,7 @@
     </row>
     <row r="4" spans="1:5" ht="36">
       <c r="A4">
-        <f t="shared" ref="A4:A16" si="0">A3+1</f>
+        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -661,39 +690,37 @@
       </c>
     </row>
     <row r="7" spans="1:5" ht="36">
-      <c r="A7">
-        <f t="shared" si="0"/>
+      <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7">
+      <c r="D7" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="36">
       <c r="A8">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E8">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="36">
@@ -701,17 +728,17 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>13</v>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="36">
@@ -720,16 +747,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E10">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="36">
@@ -738,52 +765,52 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="54">
+    <row r="12" spans="1:5" ht="36">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="54">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>4</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="36">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E13">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="36">
@@ -792,16 +819,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="36">
@@ -810,13 +837,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="E15">
         <v>4</v>
@@ -828,16 +855,93 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="36">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C17" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>9</v>
       </c>
-      <c r="E16">
-        <v>4</v>
+      <c r="E17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="36">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="E19">
+        <f>SUM(E18+E17+E16+E15+E14+E13+E12+E11+E10+E9+E8+E7+E6+E5+E4+E3+E2)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="18">
+      <c r="C21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <f>SUM(E18+E15+E10+E7+E6+E3)</f>
+        <v>21</v>
+      </c>
+      <c r="E21">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="18">
+      <c r="C22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <f>SUM(E17+E14+E11+E9+E5)</f>
+        <v>20</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="18">
+      <c r="C23" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23">
+        <f>SUM(E16+E13+E12+E8+E4+E2)</f>
+        <v>27</v>
+      </c>
+      <c r="E23">
+        <v>4.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel file change questionnumber
</commit_message>
<xml_diff>
--- a/interview/interviewScores.xlsx
+++ b/interview/interviewScores.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
   <si>
     <t>Frågor</t>
   </si>
@@ -574,7 +574,7 @@
   <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -637,7 +637,6 @@
     </row>
     <row r="4" spans="1:5" ht="36">
       <c r="A4">
-        <f t="shared" ref="A4:A17" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
@@ -655,7 +654,7 @@
     </row>
     <row r="5" spans="1:5" ht="36">
       <c r="A5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A4:A17" si="0">A4+1</f>
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -708,7 +707,7 @@
     </row>
     <row r="8" spans="1:5" ht="36">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>11</v>
@@ -726,7 +725,7 @@
     <row r="9" spans="1:5" ht="36">
       <c r="A9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -744,7 +743,7 @@
     <row r="10" spans="1:5" ht="36">
       <c r="A10">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>13</v>
@@ -762,7 +761,7 @@
     <row r="11" spans="1:5" ht="36">
       <c r="A11">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>14</v>
@@ -780,7 +779,7 @@
     <row r="12" spans="1:5" ht="36">
       <c r="A12">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>15</v>
@@ -798,7 +797,7 @@
     <row r="13" spans="1:5" ht="54">
       <c r="A13">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>16</v>
@@ -816,7 +815,7 @@
     <row r="14" spans="1:5" ht="36">
       <c r="A14">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>17</v>
@@ -834,7 +833,7 @@
     <row r="15" spans="1:5" ht="36">
       <c r="A15">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>18</v>
@@ -852,7 +851,7 @@
     <row r="16" spans="1:5" ht="36">
       <c r="A16">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>19</v>
@@ -869,8 +868,7 @@
     </row>
     <row r="17" spans="1:5" ht="36">
       <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>20</v>
@@ -887,7 +885,7 @@
     </row>
     <row r="18" spans="1:5" ht="36">
       <c r="A18">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>20</v>
@@ -902,47 +900,14 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
-      <c r="E19">
-        <f>SUM(E18+E17+E16+E15+E14+E13+E12+E11+E10+E9+E8+E7+E6+E5+E4+E3+E2)</f>
-        <v>68</v>
-      </c>
-    </row>
     <row r="21" spans="1:5" ht="18">
-      <c r="C21" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D21">
-        <f>SUM(E18+E15+E10+E7+E6+E3)</f>
-        <v>21</v>
-      </c>
-      <c r="E21">
-        <v>3.5</v>
-      </c>
+      <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:5" ht="18">
-      <c r="C22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22">
-        <f>SUM(E17+E14+E11+E9+E5)</f>
-        <v>20</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
+      <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:5" ht="18">
-      <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23">
-        <f>SUM(E16+E13+E12+E8+E4+E2)</f>
-        <v>27</v>
-      </c>
-      <c r="E23">
-        <v>4.5</v>
-      </c>
+      <c r="C23" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>